<commit_message>
Bug Fix in data_curating
</commit_message>
<xml_diff>
--- a/Reports:Notes/Results_SF.xlsx
+++ b/Reports:Notes/Results_SF.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brad/Desktop/CS6620/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brad/Desktop/CS6620/Project/Reports:Notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C2B17F-A5A7-3447-A60D-9AC1150D1434}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB150F02-F879-324D-9353-75F328665FBD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4160" yWindow="1560" windowWidth="32720" windowHeight="18640" xr2:uid="{5F3EDD50-8C15-7244-ABFC-28224EC0F5DB}"/>
+    <workbookView xWindow="-300" yWindow="1260" windowWidth="32720" windowHeight="18640" xr2:uid="{5F3EDD50-8C15-7244-ABFC-28224EC0F5DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
   <si>
     <t>KNN</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>On Total Generation, other conditions same as last</t>
+  </si>
+  <si>
+    <t>Average Generation (after bug fix) 0.85-0.15, MinMaxScale x, Quantily y, LSTM 400 epochs, ANN 500 epochs</t>
   </si>
 </sst>
 </file>
@@ -206,12 +209,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -224,6 +221,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -539,10 +542,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42175ECF-4D3D-FC44-BD25-B6FFA94718DA}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="227" zoomScaleNormal="227" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="227" zoomScaleNormal="227" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7:M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -551,18 +554,18 @@
     <col min="2" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18" thickBot="1">
-      <c r="A1" s="6"/>
-      <c r="B1" s="7" t="s">
+    <row r="1" spans="1:13" ht="18" thickBot="1">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F1" t="s">
@@ -583,8 +586,14 @@
       <c r="K1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="18" thickTop="1" thickBot="1">
+      <c r="L1" t="s">
+        <v>5</v>
+      </c>
+      <c r="M1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="18" thickTop="1" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -597,29 +606,35 @@
       <c r="D2">
         <v>0.878</v>
       </c>
-      <c r="E2" s="9">
+      <c r="E2" s="7">
         <v>0.70599999999999996</v>
       </c>
-      <c r="F2" s="9">
+      <c r="F2" s="7">
         <v>0.89600000000000002</v>
       </c>
-      <c r="G2" s="9">
+      <c r="G2" s="7">
         <v>0.60399999999999998</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="7">
         <v>0.89200000000000002</v>
       </c>
-      <c r="I2" s="9">
+      <c r="I2" s="7">
         <v>0.65500000000000003</v>
       </c>
-      <c r="J2" s="9">
+      <c r="J2" s="7">
         <v>0.76200000000000001</v>
       </c>
-      <c r="K2" s="9">
+      <c r="K2" s="7">
         <v>0.33300000000000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="17" thickBot="1">
+      <c r="L2" s="7">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="M2" s="7">
+        <v>0.60399999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="17" thickBot="1">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -632,29 +647,35 @@
       <c r="D3">
         <v>0.99</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="8">
         <v>0.76700000000000002</v>
       </c>
-      <c r="F3" s="10">
+      <c r="F3" s="8">
         <v>0.99</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="8">
         <v>0.76800000000000002</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="8">
         <v>0.98899999999999999</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="8">
         <v>0.83</v>
       </c>
-      <c r="J3" s="10">
+      <c r="J3" s="8">
         <v>0.97099999999999997</v>
       </c>
-      <c r="K3" s="10">
+      <c r="K3" s="8">
         <v>0.79900000000000004</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="17" thickBot="1">
+      <c r="L3" s="8">
+        <v>0.99</v>
+      </c>
+      <c r="M3" s="8">
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="17" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -667,29 +688,35 @@
       <c r="D4">
         <v>0.81</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="7">
         <v>0.71399999999999997</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="7">
         <v>0.93200000000000005</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="7">
         <v>0.75800000000000001</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="7">
         <v>0.92700000000000005</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="7">
         <v>0.80600000000000005</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="7">
         <v>0.79600000000000004</v>
       </c>
-      <c r="K4" s="9">
+      <c r="K4" s="7">
         <v>0.48599999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="17" thickBot="1">
+      <c r="L4" s="7">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="M4" s="7">
+        <v>0.75600000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="17" thickBot="1">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -702,29 +729,35 @@
       <c r="D5">
         <v>0.66700000000000004</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="8">
         <v>0.47299999999999998</v>
       </c>
-      <c r="F5" s="10">
+      <c r="F5" s="8">
         <v>0.68700000000000006</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="8">
         <v>0.46100000000000002</v>
       </c>
-      <c r="H5" s="10">
+      <c r="H5" s="8">
         <v>0.69099999999999995</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="8">
         <v>0.495</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="8">
         <v>0.45800000000000002</v>
       </c>
-      <c r="K5" s="10">
+      <c r="K5" s="8">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="17" thickBot="1">
+      <c r="L5" s="8">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="M5" s="8">
+        <v>0.53300000000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="17" thickBot="1">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -737,124 +770,147 @@
       <c r="D6">
         <v>-2.9980000000000002</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="7">
         <v>-2.14</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="7">
         <v>0.89800000000000002</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="7">
         <v>0.7</v>
       </c>
-      <c r="H6" s="9">
+      <c r="H6" s="7">
         <v>0.91100000000000003</v>
       </c>
-      <c r="I6" s="9">
+      <c r="I6" s="7">
         <v>0.79200000000000004</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="7">
         <v>0.69299999999999995</v>
       </c>
-      <c r="K6" s="9">
+      <c r="K6" s="7">
         <v>0.47199999999999998</v>
       </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="B7" s="5" t="s">
+      <c r="L6" s="7">
+        <v>0.91900000000000004</v>
+      </c>
+      <c r="M6" s="7">
+        <v>0.71199999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="B7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="4" t="s">
+      <c r="C7" s="9"/>
+      <c r="D7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4" t="s">
+      <c r="E7" s="10"/>
+      <c r="F7" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4" t="s">
+      <c r="G7" s="10"/>
+      <c r="H7" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4" t="s">
+      <c r="I7" s="10"/>
+      <c r="J7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="4"/>
-    </row>
-    <row r="8" spans="1:11">
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-    </row>
-    <row r="9" spans="1:11">
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-    </row>
-    <row r="10" spans="1:11">
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-    </row>
-    <row r="11" spans="1:11">
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-    </row>
-    <row r="12" spans="1:11">
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-    </row>
-    <row r="13" spans="1:11">
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="M7" s="10"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="L7:M13"/>
     <mergeCell ref="B7:C13"/>
     <mergeCell ref="D7:E13"/>
     <mergeCell ref="F7:G13"/>

</xml_diff>

<commit_message>
split data into seasons and fit random forest
</commit_message>
<xml_diff>
--- a/Reports:Notes/Results_SF.xlsx
+++ b/Reports:Notes/Results_SF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brad/Desktop/CS6620/Project/Reports:Notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB150F02-F879-324D-9353-75F328665FBD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81FD815-A1E4-F149-B82F-A61A333FF940}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-300" yWindow="1260" windowWidth="32720" windowHeight="18640" xr2:uid="{5F3EDD50-8C15-7244-ABFC-28224EC0F5DB}"/>
+    <workbookView xWindow="0" yWindow="1240" windowWidth="32720" windowHeight="18640" xr2:uid="{5F3EDD50-8C15-7244-ABFC-28224EC0F5DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t>KNN</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Average Generation (after bug fix) 0.85-0.15, MinMaxScale x, Quantily y, LSTM 400 epochs, ANN 500 epochs</t>
+  </si>
+  <si>
+    <t>Total Generation (after bug fix) 0.85 - 0.15 split Same as previous</t>
   </si>
 </sst>
 </file>
@@ -222,10 +225,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -542,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42175ECF-4D3D-FC44-BD25-B6FFA94718DA}">
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="227" zoomScaleNormal="227" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7:M13"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -554,7 +557,7 @@
     <col min="2" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18" thickBot="1">
+    <row r="1" spans="1:15" ht="18" thickBot="1">
       <c r="A1" s="4"/>
       <c r="B1" s="5" t="s">
         <v>5</v>
@@ -592,8 +595,14 @@
       <c r="M1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" ht="18" thickTop="1" thickBot="1">
+      <c r="N1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="18" thickTop="1" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -633,8 +642,14 @@
       <c r="M2" s="7">
         <v>0.60399999999999998</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="17" thickBot="1">
+      <c r="N2" s="7">
+        <v>0.76100000000000001</v>
+      </c>
+      <c r="O2" s="7">
+        <v>0.33700000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="17" thickBot="1">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -674,8 +689,14 @@
       <c r="M3" s="8">
         <v>0.79</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="17" thickBot="1">
+      <c r="N3" s="8">
+        <v>0.97099999999999997</v>
+      </c>
+      <c r="O3" s="8">
+        <v>0.48399999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="17" thickBot="1">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
@@ -715,8 +736,14 @@
       <c r="M4" s="7">
         <v>0.75600000000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="17" thickBot="1">
+      <c r="N4" s="7">
+        <v>0.79600000000000004</v>
+      </c>
+      <c r="O4" s="7">
+        <v>0.496</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="17" thickBot="1">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -757,7 +784,7 @@
         <v>0.53300000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="17" thickBot="1">
+    <row r="6" spans="1:15" ht="17" thickBot="1">
       <c r="A6" s="3" t="s">
         <v>3</v>
       </c>
@@ -798,118 +825,135 @@
         <v>0.71199999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
-      <c r="B7" s="9" t="s">
+    <row r="7" spans="1:15">
+      <c r="B7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="9"/>
-      <c r="D7" s="10" t="s">
+      <c r="C7" s="10"/>
+      <c r="D7" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10" t="s">
+      <c r="E7" s="9"/>
+      <c r="F7" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10" t="s">
+      <c r="G7" s="9"/>
+      <c r="H7" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10" t="s">
+      <c r="I7" s="9"/>
+      <c r="J7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10" t="s">
+      <c r="K7" s="9"/>
+      <c r="L7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="M7" s="10"/>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="B8" s="10"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="B10" s="10"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
-      <c r="G10" s="10"/>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10"/>
-      <c r="J10" s="10"/>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="10"/>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
+      <c r="M7" s="9"/>
+      <c r="N7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="O7" s="9"/>
+    </row>
+    <row r="8" spans="1:15">
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9"/>
+    </row>
+    <row r="9" spans="1:15">
+      <c r="B9" s="9"/>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+    </row>
+    <row r="10" spans="1:15">
+      <c r="B10" s="9"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9"/>
+      <c r="J10" s="9"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+    </row>
+    <row r="11" spans="1:15">
+      <c r="B11" s="9"/>
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+    </row>
+    <row r="12" spans="1:15">
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="9"/>
+      <c r="N13" s="9"/>
+      <c r="O13" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="N7:O13"/>
     <mergeCell ref="L7:M13"/>
     <mergeCell ref="B7:C13"/>
     <mergeCell ref="D7:E13"/>

</xml_diff>

<commit_message>
encoded sun, month, and day of year as 2d numbers
</commit_message>
<xml_diff>
--- a/Reports:Notes/Results_SF.xlsx
+++ b/Reports:Notes/Results_SF.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brad/Desktop/CS6620/Project/Reports:Notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C81FD815-A1E4-F149-B82F-A61A333FF940}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{162FF1D6-AEE6-A342-8C6C-DF9B68BEACC5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1240" windowWidth="32720" windowHeight="18640" xr2:uid="{5F3EDD50-8C15-7244-ABFC-28224EC0F5DB}"/>
+    <workbookView xWindow="40280" yWindow="2240" windowWidth="32480" windowHeight="17280" activeTab="1" xr2:uid="{5F3EDD50-8C15-7244-ABFC-28224EC0F5DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Seasons" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="47">
   <si>
     <t>KNN</t>
   </si>
@@ -82,13 +83,106 @@
   </si>
   <si>
     <t>Total Generation (after bug fix) 0.85 - 0.15 split Same as previous</t>
+  </si>
+  <si>
+    <t>tr_r2</t>
+  </si>
+  <si>
+    <t>r2</t>
+  </si>
+  <si>
+    <t>mae</t>
+  </si>
+  <si>
+    <t>mse</t>
+  </si>
+  <si>
+    <t>medianAe</t>
+  </si>
+  <si>
+    <t>val_r2</t>
+  </si>
+  <si>
+    <t>medianAE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Random Forests only </t>
+  </si>
+  <si>
+    <t>MAE</t>
+  </si>
+  <si>
+    <t>MSE</t>
+  </si>
+  <si>
+    <t>MedianAE</t>
+  </si>
+  <si>
+    <t>ExpVar</t>
+  </si>
+  <si>
+    <t>EXP description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normal </t>
+  </si>
+  <si>
+    <t>Warm Train</t>
+  </si>
+  <si>
+    <t>Warm Test</t>
+  </si>
+  <si>
+    <t>Cold Train</t>
+  </si>
+  <si>
+    <t>Cold Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sine and cos of zenith, azimuth month, day of year, drop azimuth,  zenith , elevation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Previous but, No Drop </t>
+  </si>
+  <si>
+    <t>Mean Squared Error</t>
+  </si>
+  <si>
+    <t>Mean Absolute Error</t>
+  </si>
+  <si>
+    <t>Median Absolute Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R^2 </t>
+  </si>
+  <si>
+    <t>Unsplit Train</t>
+  </si>
+  <si>
+    <t>Unsplit Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mean Percent Error (%) </t>
+  </si>
+  <si>
+    <t>RF Only</t>
+  </si>
+  <si>
+    <t>Before</t>
+  </si>
+  <si>
+    <t>Added Rolling Averages</t>
+  </si>
+  <si>
+    <t>Encoded x and y</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -111,8 +205,21 @@
       <color rgb="FF000000"/>
       <name val="CMU SERIF ROMAN"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -123,6 +230,24 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFF0F0F0"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
       </patternFill>
     </fill>
   </fills>
@@ -198,10 +323,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
@@ -225,14 +353,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
+    <cellStyle name="20% - Accent3" xfId="2" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="3" builtinId="39"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -545,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42175ECF-4D3D-FC44-BD25-B6FFA94718DA}">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="227" zoomScaleNormal="227" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -826,130 +969,302 @@
       </c>
     </row>
     <row r="7" spans="1:15">
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="9" t="s">
+      <c r="C7" s="16"/>
+      <c r="D7" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9" t="s">
+      <c r="E7" s="15"/>
+      <c r="F7" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9" t="s">
+      <c r="G7" s="15"/>
+      <c r="H7" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="9"/>
-      <c r="J7" s="9" t="s">
+      <c r="I7" s="15"/>
+      <c r="J7" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9" t="s">
+      <c r="K7" s="15"/>
+      <c r="L7" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9" t="s">
+      <c r="M7" s="15"/>
+      <c r="N7" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="O7" s="9"/>
+      <c r="O7" s="15"/>
     </row>
     <row r="8" spans="1:15">
-      <c r="B8" s="9"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="9"/>
-      <c r="E8" s="9"/>
-      <c r="F8" s="9"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9"/>
-      <c r="I8" s="9"/>
-      <c r="J8" s="9"/>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="15"/>
+      <c r="O8" s="15"/>
     </row>
     <row r="9" spans="1:15">
-      <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="L9" s="9"/>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
     </row>
     <row r="10" spans="1:15">
-      <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="15"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="15"/>
+      <c r="O10" s="15"/>
     </row>
     <row r="11" spans="1:15">
-      <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
     </row>
     <row r="12" spans="1:15">
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
+      <c r="G12" s="15"/>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="15"/>
+      <c r="O12" s="15"/>
     </row>
     <row r="13" spans="1:15">
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="15"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
+      <c r="M13" s="15"/>
+      <c r="N13" s="15"/>
+      <c r="O13" s="15"/>
+    </row>
+    <row r="14" spans="1:15" ht="17" thickBot="1">
+      <c r="B14" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" s="10"/>
+    </row>
+    <row r="15" spans="1:15" ht="18" thickTop="1" thickBot="1">
+      <c r="A15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>0.90400000000000003</v>
+      </c>
+      <c r="C15">
+        <v>6.4299999999999996E-2</v>
+      </c>
+      <c r="D15">
+        <v>8.0400000000000003E-3</v>
+      </c>
+      <c r="E15">
+        <v>4.4400000000000002E-2</v>
+      </c>
+      <c r="F15">
+        <v>0.60099999999999998</v>
+      </c>
+      <c r="G15">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="H15">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="I15">
+        <v>0.114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="17" thickBot="1">
+      <c r="A16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>0.99</v>
+      </c>
+      <c r="C16">
+        <v>1.823E-2</v>
+      </c>
+      <c r="D16">
+        <v>8.0699999999999999E-4</v>
+      </c>
+      <c r="E16">
+        <v>1.14E-2</v>
+      </c>
+      <c r="F16">
+        <v>0.79300000000000004</v>
+      </c>
+      <c r="G16">
+        <v>9.0899999999999995E-2</v>
+      </c>
+      <c r="H16">
+        <v>1.5100000000000001E-2</v>
+      </c>
+      <c r="I16">
+        <v>6.6500000000000004E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="17" thickBot="1">
+      <c r="A17" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B17">
+        <v>0.93799999999999994</v>
+      </c>
+      <c r="C17">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="D17">
+        <v>5.1599999999999997E-3</v>
+      </c>
+      <c r="E17">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="F17">
+        <v>0.69299999999999995</v>
+      </c>
+      <c r="G17">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="H17">
+        <v>2.24E-2</v>
+      </c>
+      <c r="I17">
+        <v>9.9299999999999999E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="17" thickBot="1">
+      <c r="A18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <v>0.80500000000000005</v>
+      </c>
+      <c r="C18">
+        <v>9.7100000000000006E-2</v>
+      </c>
+      <c r="D18">
+        <v>1.6199999999999999E-2</v>
+      </c>
+      <c r="E18">
+        <v>7.5600000000000001E-2</v>
+      </c>
+      <c r="F18">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="G18">
+        <v>0.151</v>
+      </c>
+      <c r="H18">
+        <v>3.5200000000000002E-2</v>
+      </c>
+      <c r="I18">
+        <v>0.128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="17" thickBot="1">
+      <c r="A19" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>0.90100000000000002</v>
+      </c>
+      <c r="C19">
+        <v>6.9199999999999998E-2</v>
+      </c>
+      <c r="D19">
+        <v>8.2299999999999995E-3</v>
+      </c>
+      <c r="E19">
+        <v>5.62E-2</v>
+      </c>
+      <c r="F19">
+        <v>0.72599999999999998</v>
+      </c>
+      <c r="G19">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="H19">
+        <v>0.02</v>
+      </c>
+      <c r="I19">
+        <v>7.4300000000000005E-2</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -963,4 +1278,846 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A49E7B-EF17-864B-A571-C69B1014F0AF}">
+  <dimension ref="A1:M44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <cols>
+    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="C2">
+        <v>0.95199999999999996</v>
+      </c>
+      <c r="D2" s="14">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="E2" s="14">
+        <v>0.78700000000000003</v>
+      </c>
+      <c r="F2">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="G2">
+        <v>0.96</v>
+      </c>
+      <c r="H2" s="14">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="I2" s="14">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="J2">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="K2">
+        <v>0.96</v>
+      </c>
+      <c r="L2" s="14">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="M2" s="14">
+        <v>0.78100000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3">
+        <v>1.4E-2</v>
+      </c>
+      <c r="C3">
+        <v>4.7600000000000003E-2</v>
+      </c>
+      <c r="D3" s="14">
+        <v>2.64E-2</v>
+      </c>
+      <c r="E3" s="14">
+        <v>9.4700000000000006E-2</v>
+      </c>
+      <c r="F3">
+        <v>1.4E-2</v>
+      </c>
+      <c r="G3">
+        <v>0.42599999999999999</v>
+      </c>
+      <c r="H3" s="14">
+        <v>2.63E-2</v>
+      </c>
+      <c r="I3" s="14">
+        <v>9.7100000000000006E-2</v>
+      </c>
+      <c r="J3">
+        <v>1.3899999999999999E-2</v>
+      </c>
+      <c r="K3">
+        <v>4.2299999999999997E-2</v>
+      </c>
+      <c r="L3" s="14">
+        <v>2.64E-2</v>
+      </c>
+      <c r="M3" s="14">
+        <v>9.6100000000000005E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4">
+        <v>5.44E-4</v>
+      </c>
+      <c r="C4">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="D4" s="14">
+        <v>1.5299999999999999E-3</v>
+      </c>
+      <c r="E4" s="14">
+        <v>1.6500000000000001E-2</v>
+      </c>
+      <c r="F4">
+        <v>5.5000000000000003E-4</v>
+      </c>
+      <c r="G4">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="H4" s="14">
+        <v>1.5E-3</v>
+      </c>
+      <c r="I4" s="14">
+        <v>1.72E-2</v>
+      </c>
+      <c r="J4">
+        <v>5.5000000000000003E-4</v>
+      </c>
+      <c r="K4">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="L4" s="14">
+        <v>1.5100000000000001E-3</v>
+      </c>
+      <c r="M4" s="14">
+        <v>1.6899999999999998E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5">
+        <v>8.7600000000000004E-3</v>
+      </c>
+      <c r="C5">
+        <v>4.0099999999999997E-2</v>
+      </c>
+      <c r="D5" s="14">
+        <v>1.7600000000000001E-2</v>
+      </c>
+      <c r="E5" s="14">
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="F5">
+        <v>8.5199999999999998E-3</v>
+      </c>
+      <c r="G5">
+        <v>3.4099999999999998E-2</v>
+      </c>
+      <c r="H5" s="14">
+        <v>1.7600000000000001E-2</v>
+      </c>
+      <c r="I5" s="14">
+        <v>7.5499999999999998E-2</v>
+      </c>
+      <c r="J5">
+        <v>8.3899999999999999E-3</v>
+      </c>
+      <c r="K5">
+        <v>3.5400000000000001E-2</v>
+      </c>
+      <c r="L5" s="14">
+        <v>0.17399999999999999</v>
+      </c>
+      <c r="M5" s="14">
+        <v>7.5899999999999995E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="C6">
+        <v>0.95960000000000001</v>
+      </c>
+      <c r="D6" s="14">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="E6" s="14">
+        <v>0.80600000000000005</v>
+      </c>
+      <c r="F6">
+        <v>0.99299999999999999</v>
+      </c>
+      <c r="G6">
+        <v>0.96099999999999997</v>
+      </c>
+      <c r="H6" s="14">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="I6" s="14">
+        <v>0.80100000000000005</v>
+      </c>
+      <c r="J6">
+        <v>0.99339999999999995</v>
+      </c>
+      <c r="K6">
+        <v>0.96099999999999997</v>
+      </c>
+      <c r="L6" s="14">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="M6" s="14">
+        <v>0.80300000000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="17"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="17"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="17"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="15"/>
+      <c r="G10" s="15"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
+      <c r="M10" s="15"/>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="17"/>
+      <c r="B11" s="18"/>
+      <c r="C11" s="18"/>
+      <c r="D11" s="18"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E14" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="C15">
+        <v>0.95</v>
+      </c>
+      <c r="D15">
+        <v>0.98</v>
+      </c>
+      <c r="E15">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="F15">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="G15">
+        <v>0.75600000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C16">
+        <v>12.1</v>
+      </c>
+      <c r="D16">
+        <v>7.74</v>
+      </c>
+      <c r="E16">
+        <v>30.1</v>
+      </c>
+      <c r="F16">
+        <v>5.29</v>
+      </c>
+      <c r="G16">
+        <v>33.1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+      <c r="B17">
+        <v>0.79400000000000004</v>
+      </c>
+      <c r="C17">
+        <v>1.88</v>
+      </c>
+      <c r="D17">
+        <v>1.48</v>
+      </c>
+      <c r="E17">
+        <v>5.39</v>
+      </c>
+      <c r="F17">
+        <v>0.96099999999999997</v>
+      </c>
+      <c r="G17">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="H17" s="12"/>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18">
+        <v>3.33</v>
+      </c>
+      <c r="C18">
+        <v>7.9</v>
+      </c>
+      <c r="D18">
+        <v>5.9</v>
+      </c>
+      <c r="E18">
+        <v>60.12</v>
+      </c>
+      <c r="F18">
+        <v>3.41</v>
+      </c>
+      <c r="G18">
+        <v>48.71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="C19">
+        <v>1.27</v>
+      </c>
+      <c r="D19">
+        <v>0.80100000000000005</v>
+      </c>
+      <c r="E19">
+        <v>3.64</v>
+      </c>
+      <c r="F19">
+        <v>0.438</v>
+      </c>
+      <c r="G19">
+        <v>2.39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" t="s">
+        <v>23</v>
+      </c>
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" t="s">
+        <v>33</v>
+      </c>
+      <c r="F22" t="s">
+        <v>40</v>
+      </c>
+      <c r="G22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B23">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="C23">
+        <v>0.95</v>
+      </c>
+      <c r="D23">
+        <v>0.98</v>
+      </c>
+      <c r="E23">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="F23">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="G23">
+        <v>0.75600000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C24">
+        <v>12.1</v>
+      </c>
+      <c r="D24">
+        <v>7.74</v>
+      </c>
+      <c r="E24">
+        <v>30.1</v>
+      </c>
+      <c r="F24">
+        <v>5.29</v>
+      </c>
+      <c r="G24">
+        <v>33.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25">
+        <v>0.79400000000000004</v>
+      </c>
+      <c r="C25">
+        <v>1.88</v>
+      </c>
+      <c r="D25">
+        <v>1.48</v>
+      </c>
+      <c r="E25">
+        <v>5.39</v>
+      </c>
+      <c r="F25">
+        <v>0.96099999999999997</v>
+      </c>
+      <c r="G25">
+        <v>4.5199999999999996</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="A26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26">
+        <v>3.33</v>
+      </c>
+      <c r="C26">
+        <v>7.9</v>
+      </c>
+      <c r="D26">
+        <v>5.9</v>
+      </c>
+      <c r="E26">
+        <v>60.12</v>
+      </c>
+      <c r="F26">
+        <v>3.41</v>
+      </c>
+      <c r="G26">
+        <v>48.71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="C27">
+        <v>1.27</v>
+      </c>
+      <c r="D27">
+        <v>0.80100000000000005</v>
+      </c>
+      <c r="E27">
+        <v>3.64</v>
+      </c>
+      <c r="F27">
+        <v>0.438</v>
+      </c>
+      <c r="G27">
+        <v>2.39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="A30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" t="s">
+        <v>42</v>
+      </c>
+      <c r="D30" t="s">
+        <v>37</v>
+      </c>
+      <c r="E30" t="s">
+        <v>36</v>
+      </c>
+      <c r="F30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="C31">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D31">
+        <v>0.79400000000000004</v>
+      </c>
+      <c r="E31">
+        <v>3.33</v>
+      </c>
+      <c r="F31">
+        <v>0.29399999999999998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32">
+        <v>0.95</v>
+      </c>
+      <c r="C32">
+        <v>12.1</v>
+      </c>
+      <c r="D32">
+        <v>1.88</v>
+      </c>
+      <c r="E32">
+        <v>7.9</v>
+      </c>
+      <c r="F32">
+        <v>1.27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+      <c r="B33">
+        <v>0.98</v>
+      </c>
+      <c r="C33">
+        <v>7.74</v>
+      </c>
+      <c r="D33">
+        <v>1.48</v>
+      </c>
+      <c r="E33">
+        <v>5.9</v>
+      </c>
+      <c r="F33">
+        <v>0.80100000000000005</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>0.77500000000000002</v>
+      </c>
+      <c r="C34">
+        <v>30.1</v>
+      </c>
+      <c r="D34">
+        <v>5.39</v>
+      </c>
+      <c r="E34">
+        <v>60.12</v>
+      </c>
+      <c r="F34">
+        <v>3.64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>40</v>
+      </c>
+      <c r="B35">
+        <v>0.98699999999999999</v>
+      </c>
+      <c r="C35">
+        <v>5.29</v>
+      </c>
+      <c r="D35">
+        <v>0.96099999999999997</v>
+      </c>
+      <c r="E35">
+        <v>3.41</v>
+      </c>
+      <c r="F35">
+        <v>0.438</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>41</v>
+      </c>
+      <c r="B36">
+        <v>0.75600000000000001</v>
+      </c>
+      <c r="C36">
+        <v>33.1</v>
+      </c>
+      <c r="D36">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="E36">
+        <v>48.71</v>
+      </c>
+      <c r="F36">
+        <v>2.39</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" t="s">
+        <v>43</v>
+      </c>
+      <c r="B40" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" t="s">
+        <v>45</v>
+      </c>
+      <c r="D40" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" t="s">
+        <v>30</v>
+      </c>
+      <c r="B41">
+        <v>4.2699999999999996</v>
+      </c>
+      <c r="C41">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="D41">
+        <v>4.0999999999999996</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>31</v>
+      </c>
+      <c r="B42">
+        <v>13.9</v>
+      </c>
+      <c r="C42">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="D42">
+        <v>12.1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>32</v>
+      </c>
+      <c r="B43">
+        <v>7.78</v>
+      </c>
+      <c r="C43">
+        <v>7.81</v>
+      </c>
+      <c r="D43">
+        <v>7.74</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" t="s">
+        <v>33</v>
+      </c>
+      <c r="B44">
+        <v>29.8</v>
+      </c>
+      <c r="C44">
+        <v>29.6</v>
+      </c>
+      <c r="D44">
+        <v>30.1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A7:A11"/>
+    <mergeCell ref="B7:E11"/>
+    <mergeCell ref="F7:I11"/>
+    <mergeCell ref="J7:M11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added readme to src and Data folders
</commit_message>
<xml_diff>
--- a/Reports:Notes/Results_SF.xlsx
+++ b/Reports:Notes/Results_SF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brad/Desktop/CS6620/Project/Reports:Notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0626E702-B260-E045-B2C6-D6E320D72358}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689FFD56-72F2-0542-8EBB-A78A0D311C78}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48620" yWindow="8840" windowWidth="32480" windowHeight="17280" activeTab="1" xr2:uid="{5F3EDD50-8C15-7244-ABFC-28224EC0F5DB}"/>
+    <workbookView xWindow="3700" yWindow="1800" windowWidth="32480" windowHeight="17280" activeTab="1" xr2:uid="{5F3EDD50-8C15-7244-ABFC-28224EC0F5DB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1314,7 +1314,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69A49E7B-EF17-864B-A571-C69B1014F0AF}">
   <dimension ref="A1:M71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B7" sqref="B7:E11"/>
     </sheetView>
   </sheetViews>
@@ -2683,13 +2683,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="J7:M11"/>
+    <mergeCell ref="A47:E47"/>
     <mergeCell ref="A56:E56"/>
     <mergeCell ref="A65:E65"/>
     <mergeCell ref="A7:A11"/>
     <mergeCell ref="B7:E11"/>
     <mergeCell ref="F7:I11"/>
-    <mergeCell ref="J7:M11"/>
-    <mergeCell ref="A47:E47"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>